<commit_message>
burndown and retrospective report added
</commit_message>
<xml_diff>
--- a/Sprint 2 Documentation/ProductBacklog.xlsx
+++ b/Sprint 2 Documentation/ProductBacklog.xlsx
@@ -1,29 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2206\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni - gitfolder\Agile-Software-Development\Sprint 2 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BAD7A59-D85E-4996-B05E-54E872DABD7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276459CB-095E-4688-8267-4F8FA7F7C055}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="49">
   <si>
     <t>User Story ID</t>
   </si>
@@ -175,13 +173,16 @@
   </si>
   <si>
     <t>best match - a self made formula comparing price to distance</t>
+  </si>
+  <si>
+    <t>OUT OF REACH(AXED)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,26 +635,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ40"/>
+  <dimension ref="A1:BJ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="62.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="62.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="15">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -682,7 +683,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="15">
+    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="C2" s="4" t="s">
         <v>9</v>
@@ -698,7 +699,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -725,7 +726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -752,7 +753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -779,7 +780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -806,7 +807,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8</v>
       </c>
@@ -833,7 +834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9</v>
       </c>
@@ -860,7 +861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12</v>
       </c>
@@ -887,7 +888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -914,7 +915,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -941,7 +942,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>13</v>
       </c>
@@ -968,7 +969,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -995,7 +996,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>16</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:62" s="3" customFormat="1" ht="15">
+    <row r="18" spans="1:62" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:62" s="8" customFormat="1" ht="15">
+    <row r="19" spans="1:62" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="6" t="s">
@@ -1178,7 +1179,7 @@
       <c r="BI19" s="7"/>
       <c r="BJ19" s="7"/>
     </row>
-    <row r="20" spans="1:62" ht="15">
+    <row r="20" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:62" ht="15">
+    <row r="21" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:62" ht="15">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1259,7 +1260,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:62" ht="15">
+    <row r="23" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1279,14 +1280,14 @@
         <v>1</v>
       </c>
       <c r="H23" s="17">
-        <f t="shared" ref="H23:H32" si="2">(F23/G23)</f>
+        <f t="shared" ref="H23:H33" si="2">(F23/G23)</f>
         <v>4</v>
       </c>
       <c r="I23" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:62" ht="15">
+    <row r="24" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>11</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:62" ht="15">
+    <row r="25" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>17</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:62" ht="15">
+    <row r="26" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>19</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:62" ht="15">
+    <row r="27" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:62" ht="15">
+    <row r="28" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>18</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:62" ht="15">
+    <row r="29" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:62" ht="15">
+    <row r="30" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:62" ht="15">
+    <row r="31" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>15</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:62" ht="15">
+    <row r="32" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>21</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>42</v>
       </c>
       <c r="D32" s="21">
-        <v>43923</v>
+        <v>43892</v>
       </c>
       <c r="E32" s="21">
         <v>43984</v>
@@ -1529,44 +1530,72 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15">
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" ht="15">
-      <c r="B34" s="9" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" s="18">
+        <v>4</v>
+      </c>
+      <c r="G33" s="18">
+        <v>3</v>
+      </c>
+      <c r="H33" s="17">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="2"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="17"/>
-    </row>
-    <row r="35" spans="2:8" ht="15">
-      <c r="B35" t="s">
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="15">
-      <c r="B36" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15">
-      <c r="B37" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15">
-      <c r="B38" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15"/>
-    <row r="40" spans="2:8" ht="15"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:I31">
     <sortCondition descending="1" ref="F20:F31"/>
     <sortCondition ref="G20:G31"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I2 I35:I1048576 I18:I19" xr:uid="{1E6226B8-A8D1-4D7A-9B0F-FAA90AAF118D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I2 I36:I1048576 I18:I19" xr:uid="{1E6226B8-A8D1-4D7A-9B0F-FAA90AAF118D}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1579,7 +1608,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I16 I20:I34</xm:sqref>
+          <xm:sqref>I3:I16 I20:I35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1593,22 +1622,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>